<commit_message>
update the directed graph function
</commit_message>
<xml_diff>
--- a/grid_data_sheet.xlsx
+++ b/grid_data_sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mingreico\Masterthesis\-Probability-analysis-of-distance-protection-system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD8D2A9F-79EC-4737-8477-4240BA642CD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0D705BF-AA96-421A-A3A8-0AA601753576}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="14914" tabRatio="826" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="55695" yWindow="0" windowWidth="12810" windowHeight="15135" tabRatio="826" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bus_data" sheetId="1" r:id="rId1"/>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{712727A4-7FFE-4A26-AA39-947AE959215E}">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -1019,7 +1019,7 @@
         <v>1.5</v>
       </c>
       <c r="L2" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
@@ -1030,10 +1030,10 @@
         <v>0</v>
       </c>
       <c r="C3" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D3" s="1">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E3" s="1">
         <v>3.3392499999999999E-2</v>
@@ -1065,13 +1065,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D4" s="1">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="E4" s="1">
         <v>3.3392499999999999E-2</v>
@@ -1106,7 +1106,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D5" s="1">
         <v>40</v>
@@ -1144,10 +1144,10 @@
         <v>1</v>
       </c>
       <c r="C6" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6" s="1">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="E6" s="1">
         <v>3.3392499999999999E-2</v>
@@ -1179,13 +1179,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D7" s="1">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="E7" s="1">
         <v>3.3392499999999999E-2</v>
@@ -1217,13 +1217,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="2">
+        <v>2</v>
+      </c>
+      <c r="C8" s="2">
         <v>6</v>
       </c>
-      <c r="C8" s="2">
-        <v>7</v>
-      </c>
       <c r="D8" s="1">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="E8" s="1">
         <v>3.3392499999999999E-2</v>
@@ -1255,13 +1255,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="2">
+        <v>6</v>
+      </c>
+      <c r="C9" s="2">
         <v>7</v>
       </c>
-      <c r="C9" s="2">
-        <v>8</v>
-      </c>
       <c r="D9" s="1">
-        <v>0.5</v>
+        <v>15</v>
       </c>
       <c r="E9" s="1">
         <v>3.3392499999999999E-2</v>
@@ -1293,13 +1293,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="2">
+        <v>7</v>
+      </c>
+      <c r="C10" s="2">
         <v>8</v>
       </c>
-      <c r="C10" s="2">
-        <v>9</v>
-      </c>
       <c r="D10" s="1">
-        <v>5</v>
+        <v>0.5</v>
       </c>
       <c r="E10" s="1">
         <v>3.3392499999999999E-2</v>
@@ -1331,13 +1331,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="2">
+        <v>8</v>
+      </c>
+      <c r="C11" s="2">
         <v>9</v>
       </c>
-      <c r="C11" s="2">
-        <v>10</v>
-      </c>
       <c r="D11" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E11" s="1">
         <v>3.3392499999999999E-2</v>
@@ -1369,13 +1369,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="2">
+        <v>9</v>
+      </c>
+      <c r="C12" s="2">
         <v>10</v>
       </c>
-      <c r="C12" s="2">
-        <v>3</v>
-      </c>
       <c r="D12" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E12" s="1">
         <v>3.3392499999999999E-2</v>
@@ -1407,13 +1407,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="2">
+        <v>10</v>
+      </c>
+      <c r="C13" s="2">
         <v>3</v>
       </c>
-      <c r="C13" s="2">
-        <v>4</v>
-      </c>
       <c r="D13" s="1">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="E13" s="1">
         <v>3.3392499999999999E-2</v>
@@ -1445,13 +1445,13 @@
         <v>12</v>
       </c>
       <c r="B14" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C14" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D14" s="1">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E14" s="1">
         <v>3.3392499999999999E-2</v>
@@ -1475,6 +1475,44 @@
         <v>1.5</v>
       </c>
       <c r="L14" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" s="2">
+        <v>4</v>
+      </c>
+      <c r="C15" s="2">
+        <v>5</v>
+      </c>
+      <c r="D15" s="1">
+        <v>35</v>
+      </c>
+      <c r="E15" s="1">
+        <v>3.3392499999999999E-2</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0.26002459999999999</v>
+      </c>
+      <c r="G15" s="1">
+        <v>1.365E-8</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0.11815589999999999</v>
+      </c>
+      <c r="I15" s="1">
+        <v>0.97861880000000001</v>
+      </c>
+      <c r="J15" s="1">
+        <v>5.4800000000000001E-9</v>
+      </c>
+      <c r="K15" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="L15" s="2">
         <v>1</v>
       </c>
     </row>
@@ -1759,10 +1797,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2718F857-12AB-400A-82B0-10245BE084C6}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -1789,7 +1827,7 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -1803,7 +1841,7 @@
         <v>4</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -1842,10 +1880,10 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -1859,147 +1897,175 @@
         <v>1</v>
       </c>
       <c r="D7">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B8">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C8">
         <v>4</v>
       </c>
       <c r="D8">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B9">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C9">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D9">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B10">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D10">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B11">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D11">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B12">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C12">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D12">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B13">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C13">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D13">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <v>10</v>
+      </c>
+      <c r="C14">
+        <v>4</v>
+      </c>
+      <c r="D14">
         <v>12</v>
-      </c>
-      <c r="B14">
-        <v>12</v>
-      </c>
-      <c r="C14">
-        <v>3</v>
-      </c>
-      <c r="D14">
-        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B15">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D15">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16">
+        <v>12</v>
+      </c>
+      <c r="B16">
+        <v>12</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16">
         <v>14</v>
-      </c>
-      <c r="B16">
-        <v>14</v>
-      </c>
-      <c r="C16">
-        <v>2</v>
-      </c>
-      <c r="D16">
-        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17">
+        <v>13</v>
+      </c>
+      <c r="B17">
+        <v>13</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>14</v>
+      </c>
+      <c r="B18">
+        <v>14</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19">
         <v>15</v>
       </c>
-      <c r="B17">
+      <c r="B19">
         <v>15</v>
       </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17">
-        <v>2</v>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -2010,10 +2076,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F44E0D7-8D9E-42FB-A620-E40C5236102D}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K37" sqref="K37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -2040,7 +2106,7 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -2054,7 +2120,7 @@
         <v>4</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -2093,10 +2159,10 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -2110,7 +2176,7 @@
         <v>1</v>
       </c>
       <c r="D7">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -2124,7 +2190,7 @@
         <v>4</v>
       </c>
       <c r="D8">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -2135,10 +2201,10 @@
         <v>7</v>
       </c>
       <c r="C9">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D9">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -2149,10 +2215,10 @@
         <v>8</v>
       </c>
       <c r="C10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D10">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -2163,10 +2229,10 @@
         <v>9</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D11">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -2177,10 +2243,10 @@
         <v>10</v>
       </c>
       <c r="C12">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D12">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
@@ -2191,10 +2257,10 @@
         <v>11</v>
       </c>
       <c r="C13">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D13">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
@@ -2205,10 +2271,10 @@
         <v>12</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D14">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
@@ -2219,10 +2285,10 @@
         <v>13</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D15">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
@@ -2233,10 +2299,10 @@
         <v>14</v>
       </c>
       <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
         <v>3</v>
-      </c>
-      <c r="D16">
-        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
@@ -2247,10 +2313,10 @@
         <v>15</v>
       </c>
       <c r="C17">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D17">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
@@ -2261,10 +2327,10 @@
         <v>16</v>
       </c>
       <c r="C18">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D18">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
@@ -2275,10 +2341,10 @@
         <v>17</v>
       </c>
       <c r="C19">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D19">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
@@ -2289,10 +2355,10 @@
         <v>18</v>
       </c>
       <c r="C20">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D20">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
@@ -2303,10 +2369,10 @@
         <v>19</v>
       </c>
       <c r="C21">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D21">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
@@ -2317,10 +2383,10 @@
         <v>20</v>
       </c>
       <c r="C22">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D22">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
@@ -2331,10 +2397,10 @@
         <v>21</v>
       </c>
       <c r="C23">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D23">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
@@ -2345,10 +2411,10 @@
         <v>22</v>
       </c>
       <c r="C24">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D24">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
@@ -2359,10 +2425,10 @@
         <v>23</v>
       </c>
       <c r="C25">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D25">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
@@ -2373,10 +2439,10 @@
         <v>24</v>
       </c>
       <c r="C26">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D26">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
@@ -2387,10 +2453,38 @@
         <v>25</v>
       </c>
       <c r="C27">
+        <v>6</v>
+      </c>
+      <c r="D27">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <v>26</v>
+      </c>
+      <c r="C28">
+        <v>6</v>
+      </c>
+      <c r="D28">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>27</v>
+      </c>
+      <c r="C29">
         <v>2</v>
       </c>
-      <c r="D27">
-        <v>5</v>
+      <c r="D29">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add function to adapt pd parameters from external and also fix the problem of parallel line hard-coded for now
</commit_message>
<xml_diff>
--- a/grid_data_sheet.xlsx
+++ b/grid_data_sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Masterthesis\IEET\pycharmtest\backup_code_masterthesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B53FDE-17AE-44F8-B187-A8239FBAE71B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47825460-8373-4C7C-9F56-15EA613A7461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15264" yWindow="0" windowWidth="15552" windowHeight="16656" tabRatio="826" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" tabRatio="826" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bus_data" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="66">
   <si>
     <t>vn_kv</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -88,10 +88,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>"b"</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>name</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -136,10 +132,6 @@
     <t>"CD_inter5"</t>
   </si>
   <si>
-    <t>"n"</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>geodata</t>
   </si>
   <si>
@@ -281,6 +273,17 @@
   </si>
   <si>
     <t>NaN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>b</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>n</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -615,16 +618,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="A1:E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -632,13 +635,13 @@
         <v>12</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -646,16 +649,16 @@
         <v>110</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -663,16 +666,16 @@
         <v>110</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -680,16 +683,16 @@
         <v>110</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -697,16 +700,16 @@
         <v>110</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -714,16 +717,16 @@
         <v>110</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -731,16 +734,16 @@
         <v>110</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -748,16 +751,16 @@
         <v>110</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>26</v>
+        <v>65</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -765,16 +768,16 @@
         <v>110</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>26</v>
+        <v>64</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -782,16 +785,16 @@
         <v>110</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>26</v>
+        <v>64</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -799,16 +802,16 @@
         <v>110</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>26</v>
+        <v>64</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -816,19 +819,19 @@
         <v>110</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>26</v>
+        <v>64</v>
       </c>
       <c r="D12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E12" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C14" s="1"/>
     </row>
   </sheetData>
@@ -845,26 +848,26 @@
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" t="s">
         <v>39</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
         <v>40</v>
       </c>
-      <c r="D1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -879,13 +882,13 @@
         <v>65.736821035772635</v>
       </c>
       <c r="E2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F2">
         <v>0.95</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -900,13 +903,13 @@
         <v>65.736821035772635</v>
       </c>
       <c r="E3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F3">
         <v>0.95</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -921,7 +924,7 @@
         <v>32.868410517886318</v>
       </c>
       <c r="E4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F4">
         <v>0.95</v>
@@ -937,27 +940,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{712727A4-7FFE-4A26-AA39-947AE959215E}">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>10</v>
       </c>
@@ -992,7 +995,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1030,7 +1033,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1068,7 +1071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1106,7 +1109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1144,7 +1147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1182,7 +1185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1220,7 +1223,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1258,7 +1261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1296,7 +1299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1334,7 +1337,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1372,7 +1375,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1410,7 +1413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1448,7 +1451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1486,7 +1489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1538,29 +1541,29 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" t="s">
         <v>39</v>
       </c>
-      <c r="C1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D1" t="s">
-        <v>41</v>
-      </c>
       <c r="E1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1577,10 +1580,10 @@
         <v>35</v>
       </c>
       <c r="F2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1597,10 +1600,10 @@
         <v>50</v>
       </c>
       <c r="F3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1617,10 +1620,10 @@
         <v>50</v>
       </c>
       <c r="F4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1637,10 +1640,10 @@
         <v>35</v>
       </c>
       <c r="F5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1657,10 +1660,10 @@
         <v>20</v>
       </c>
       <c r="F6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1677,10 +1680,10 @@
         <v>75</v>
       </c>
       <c r="F7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1697,7 +1700,7 @@
         <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1712,7 +1715,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1727,29 +1730,29 @@
       <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
         <v>46</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>47</v>
       </c>
-      <c r="E1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1764,7 +1767,7 @@
         <v>1.7481</v>
       </c>
       <c r="E2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F2">
         <v>110</v>
@@ -1773,7 +1776,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1788,7 +1791,7 @@
         <v>1.4616</v>
       </c>
       <c r="E3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F3">
         <v>110</v>
@@ -1811,27 +1814,27 @@
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" t="s">
         <v>60</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>61</v>
       </c>
-      <c r="D1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1845,10 +1848,10 @@
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1862,10 +1865,10 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1879,10 +1882,10 @@
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1896,10 +1899,10 @@
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1913,10 +1916,10 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1930,10 +1933,10 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1947,10 +1950,10 @@
         <v>4</v>
       </c>
       <c r="E8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1964,10 +1967,10 @@
         <v>4</v>
       </c>
       <c r="E9" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1981,10 +1984,10 @@
         <v>13</v>
       </c>
       <c r="E10" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1998,10 +2001,10 @@
         <v>13</v>
       </c>
       <c r="E11" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2015,10 +2018,10 @@
         <v>5</v>
       </c>
       <c r="E12" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -2032,10 +2035,10 @@
         <v>5</v>
       </c>
       <c r="E13" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -2049,10 +2052,10 @@
         <v>12</v>
       </c>
       <c r="E14" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
@@ -2066,10 +2069,10 @@
         <v>12</v>
       </c>
       <c r="E15" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
@@ -2086,7 +2089,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2103,7 +2106,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
@@ -2117,10 +2120,10 @@
         <v>3</v>
       </c>
       <c r="E18" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
@@ -2134,7 +2137,7 @@
         <v>3</v>
       </c>
       <c r="E19" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -2152,20 +2155,20 @@
       <selection activeCell="I19" sqref="F2:I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" t="s">
         <v>60</v>
       </c>
-      <c r="C1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2179,7 +2182,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2193,7 +2196,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2207,7 +2210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2221,7 +2224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -2235,7 +2238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -2249,7 +2252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -2263,7 +2266,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -2277,7 +2280,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -2291,7 +2294,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2305,7 +2308,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2319,7 +2322,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -2333,7 +2336,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -2347,7 +2350,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
@@ -2361,7 +2364,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
@@ -2375,7 +2378,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2389,7 +2392,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
@@ -2403,7 +2406,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
@@ -2417,7 +2420,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
@@ -2431,7 +2434,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>19</v>
       </c>
@@ -2445,7 +2448,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
@@ -2459,7 +2462,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>21</v>
       </c>
@@ -2473,7 +2476,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>22</v>
       </c>
@@ -2487,7 +2490,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>23</v>
       </c>
@@ -2501,7 +2504,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>24</v>
       </c>
@@ -2515,7 +2518,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>25</v>
       </c>
@@ -2529,7 +2532,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>26</v>
       </c>
@@ -2543,7 +2546,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
fix the problem nf
</commit_message>
<xml_diff>
--- a/grid_data_sheet.xlsx
+++ b/grid_data_sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Masterthesis\IEET\pycharmtest\backup_code_masterthesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47825460-8373-4C7C-9F56-15EA613A7461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2838F9A9-053E-4256-914D-6C13BF2FC4BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" tabRatio="826" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" tabRatio="826" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bus_data" sheetId="1" r:id="rId1"/>
@@ -618,16 +618,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -641,7 +641,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -658,7 +658,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -675,7 +675,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -692,7 +692,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -709,7 +709,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -726,7 +726,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -743,7 +743,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -760,7 +760,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -777,7 +777,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -794,7 +794,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -811,7 +811,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -828,10 +828,10 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C14" s="1"/>
     </row>
   </sheetData>
@@ -848,9 +848,9 @@
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>37</v>
       </c>
@@ -867,7 +867,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -888,7 +888,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -909,7 +909,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -938,29 +938,29 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{712727A4-7FFE-4A26-AA39-947AE959215E}">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>10</v>
       </c>
@@ -995,7 +995,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1015,7 +1015,8 @@
         <v>0.26002459999999999</v>
       </c>
       <c r="G2" s="1">
-        <v>1.365E-8</v>
+        <f>0.00000001365*1000000000</f>
+        <v>13.65</v>
       </c>
       <c r="H2" s="1">
         <v>0.11815589999999999</v>
@@ -1024,7 +1025,7 @@
         <v>0.97861880000000001</v>
       </c>
       <c r="J2" s="1">
-        <v>5.4800000000000001E-9</v>
+        <v>5.48</v>
       </c>
       <c r="K2" s="1">
         <v>1.5</v>
@@ -1032,8 +1033,9 @@
       <c r="L2" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M2" s="1"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1053,7 +1055,7 @@
         <v>0.26002459999999999</v>
       </c>
       <c r="G3" s="1">
-        <v>1.365E-8</v>
+        <v>13.65</v>
       </c>
       <c r="H3" s="1">
         <v>0.11815589999999999</v>
@@ -1062,7 +1064,7 @@
         <v>0.97861880000000001</v>
       </c>
       <c r="J3" s="1">
-        <v>5.4800000000000001E-9</v>
+        <v>5.48</v>
       </c>
       <c r="K3" s="1">
         <v>1.5</v>
@@ -1070,8 +1072,9 @@
       <c r="L3" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M3" s="1"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1091,7 +1094,7 @@
         <v>0.26002459999999999</v>
       </c>
       <c r="G4" s="1">
-        <v>1.365E-8</v>
+        <v>13.65</v>
       </c>
       <c r="H4" s="1">
         <v>0.11815589999999999</v>
@@ -1100,7 +1103,7 @@
         <v>0.97861880000000001</v>
       </c>
       <c r="J4" s="1">
-        <v>5.4800000000000001E-9</v>
+        <v>5.48</v>
       </c>
       <c r="K4" s="1">
         <v>1.5</v>
@@ -1108,8 +1111,9 @@
       <c r="L4" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M4" s="1"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1129,7 +1133,7 @@
         <v>0.26002459999999999</v>
       </c>
       <c r="G5" s="1">
-        <v>1.365E-8</v>
+        <v>13.65</v>
       </c>
       <c r="H5" s="1">
         <v>0.11815589999999999</v>
@@ -1138,7 +1142,7 @@
         <v>0.97861880000000001</v>
       </c>
       <c r="J5" s="1">
-        <v>5.4800000000000001E-9</v>
+        <v>5.48</v>
       </c>
       <c r="K5" s="1">
         <v>1.5</v>
@@ -1146,8 +1150,9 @@
       <c r="L5" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M5" s="1"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1167,7 +1172,7 @@
         <v>0.26002459999999999</v>
       </c>
       <c r="G6" s="1">
-        <v>1.365E-8</v>
+        <v>13.65</v>
       </c>
       <c r="H6" s="1">
         <v>0.11815589999999999</v>
@@ -1176,7 +1181,7 @@
         <v>0.97861880000000001</v>
       </c>
       <c r="J6" s="1">
-        <v>5.4800000000000001E-9</v>
+        <v>5.48</v>
       </c>
       <c r="K6" s="1">
         <v>1.5</v>
@@ -1184,8 +1189,9 @@
       <c r="L6" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M6" s="1"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1205,7 +1211,7 @@
         <v>0.26002459999999999</v>
       </c>
       <c r="G7" s="1">
-        <v>1.365E-8</v>
+        <v>13.65</v>
       </c>
       <c r="H7" s="1">
         <v>0.11815589999999999</v>
@@ -1214,7 +1220,7 @@
         <v>0.97861880000000001</v>
       </c>
       <c r="J7" s="1">
-        <v>5.4800000000000001E-9</v>
+        <v>5.48</v>
       </c>
       <c r="K7" s="1">
         <v>1.5</v>
@@ -1222,8 +1228,9 @@
       <c r="L7" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M7" s="1"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1243,7 +1250,7 @@
         <v>0.26002459999999999</v>
       </c>
       <c r="G8" s="1">
-        <v>1.365E-8</v>
+        <v>13.65</v>
       </c>
       <c r="H8" s="1">
         <v>0.11815589999999999</v>
@@ -1252,7 +1259,7 @@
         <v>0.97861880000000001</v>
       </c>
       <c r="J8" s="1">
-        <v>5.4800000000000001E-9</v>
+        <v>5.48</v>
       </c>
       <c r="K8" s="1">
         <v>1.5</v>
@@ -1260,8 +1267,9 @@
       <c r="L8" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M8" s="1"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1281,7 +1289,7 @@
         <v>0.26002459999999999</v>
       </c>
       <c r="G9" s="1">
-        <v>1.365E-8</v>
+        <v>13.65</v>
       </c>
       <c r="H9" s="1">
         <v>0.11815589999999999</v>
@@ -1290,7 +1298,7 @@
         <v>0.97861880000000001</v>
       </c>
       <c r="J9" s="1">
-        <v>5.4800000000000001E-9</v>
+        <v>5.48</v>
       </c>
       <c r="K9" s="1">
         <v>1.5</v>
@@ -1298,8 +1306,9 @@
       <c r="L9" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M9" s="1"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1319,7 +1328,7 @@
         <v>0.26002459999999999</v>
       </c>
       <c r="G10" s="1">
-        <v>1.365E-8</v>
+        <v>13.65</v>
       </c>
       <c r="H10" s="1">
         <v>0.11815589999999999</v>
@@ -1328,7 +1337,7 @@
         <v>0.97861880000000001</v>
       </c>
       <c r="J10" s="1">
-        <v>5.4800000000000001E-9</v>
+        <v>5.48</v>
       </c>
       <c r="K10" s="1">
         <v>1.5</v>
@@ -1336,8 +1345,9 @@
       <c r="L10" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M10" s="1"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1357,7 +1367,7 @@
         <v>0.26002459999999999</v>
       </c>
       <c r="G11" s="1">
-        <v>1.365E-8</v>
+        <v>13.65</v>
       </c>
       <c r="H11" s="1">
         <v>0.11815589999999999</v>
@@ -1366,7 +1376,7 @@
         <v>0.97861880000000001</v>
       </c>
       <c r="J11" s="1">
-        <v>5.4800000000000001E-9</v>
+        <v>5.48</v>
       </c>
       <c r="K11" s="1">
         <v>1.5</v>
@@ -1374,8 +1384,9 @@
       <c r="L11" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M11" s="1"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1395,7 +1406,7 @@
         <v>0.26002459999999999</v>
       </c>
       <c r="G12" s="1">
-        <v>1.365E-8</v>
+        <v>13.65</v>
       </c>
       <c r="H12" s="1">
         <v>0.11815589999999999</v>
@@ -1404,7 +1415,7 @@
         <v>0.97861880000000001</v>
       </c>
       <c r="J12" s="1">
-        <v>5.4800000000000001E-9</v>
+        <v>5.48</v>
       </c>
       <c r="K12" s="1">
         <v>1.5</v>
@@ -1412,8 +1423,9 @@
       <c r="L12" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M12" s="1"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1433,7 +1445,7 @@
         <v>0.26002459999999999</v>
       </c>
       <c r="G13" s="1">
-        <v>1.365E-8</v>
+        <v>13.65</v>
       </c>
       <c r="H13" s="1">
         <v>0.11815589999999999</v>
@@ -1442,7 +1454,7 @@
         <v>0.97861880000000001</v>
       </c>
       <c r="J13" s="1">
-        <v>5.4800000000000001E-9</v>
+        <v>5.48</v>
       </c>
       <c r="K13" s="1">
         <v>1.5</v>
@@ -1450,8 +1462,9 @@
       <c r="L13" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M13" s="1"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1471,7 +1484,7 @@
         <v>0.26002459999999999</v>
       </c>
       <c r="G14" s="1">
-        <v>1.365E-8</v>
+        <v>13.65</v>
       </c>
       <c r="H14" s="1">
         <v>0.11815589999999999</v>
@@ -1480,7 +1493,7 @@
         <v>0.97861880000000001</v>
       </c>
       <c r="J14" s="1">
-        <v>5.4800000000000001E-9</v>
+        <v>5.48</v>
       </c>
       <c r="K14" s="1">
         <v>1.5</v>
@@ -1488,8 +1501,9 @@
       <c r="L14" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M14" s="1"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1509,7 +1523,7 @@
         <v>0.26002459999999999</v>
       </c>
       <c r="G15" s="1">
-        <v>1.365E-8</v>
+        <v>13.65</v>
       </c>
       <c r="H15" s="1">
         <v>0.11815589999999999</v>
@@ -1518,7 +1532,7 @@
         <v>0.97861880000000001</v>
       </c>
       <c r="J15" s="1">
-        <v>5.4800000000000001E-9</v>
+        <v>5.48</v>
       </c>
       <c r="K15" s="1">
         <v>1.5</v>
@@ -1526,6 +1540,7 @@
       <c r="L15" s="2">
         <v>1</v>
       </c>
+      <c r="M15" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1541,12 +1556,12 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>37</v>
       </c>
@@ -1563,7 +1578,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1583,7 +1598,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1603,7 +1618,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1623,7 +1638,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1643,7 +1658,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1663,7 +1678,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1683,7 +1698,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1715,7 +1730,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1730,9 +1745,9 @@
       <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>37</v>
       </c>
@@ -1752,7 +1767,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1776,7 +1791,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1814,13 +1829,13 @@
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>58</v>
       </c>
@@ -1834,7 +1849,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1851,7 +1866,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1868,7 +1883,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1885,7 +1900,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1902,7 +1917,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1919,7 +1934,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1936,7 +1951,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1953,7 +1968,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1970,7 +1985,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1987,7 +2002,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2004,7 +2019,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2021,7 +2036,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -2038,7 +2053,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -2055,7 +2070,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -2072,7 +2087,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -2089,7 +2104,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2106,7 +2121,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -2123,7 +2138,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -2155,9 +2170,9 @@
       <selection activeCell="I19" sqref="F2:I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>58</v>
       </c>
@@ -2168,7 +2183,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2182,7 +2197,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2196,7 +2211,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2210,7 +2225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2224,7 +2239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -2238,7 +2253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -2252,7 +2267,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -2266,7 +2281,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -2280,7 +2295,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -2294,7 +2309,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2308,7 +2323,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2322,7 +2337,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -2336,7 +2351,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -2350,7 +2365,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -2364,7 +2379,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -2378,7 +2393,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2392,7 +2407,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -2406,7 +2421,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -2420,7 +2435,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -2434,7 +2449,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -2448,7 +2463,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
@@ -2462,7 +2477,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
@@ -2476,7 +2491,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
@@ -2490,7 +2505,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
@@ -2504,7 +2519,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
@@ -2518,7 +2533,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
@@ -2532,7 +2547,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
@@ -2546,7 +2561,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>

</xml_diff>